<commit_message>
misc files from work pc
</commit_message>
<xml_diff>
--- a/data/calc.xlsx
+++ b/data/calc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="23955" windowHeight="11055"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="23955" windowHeight="11055" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="272">
   <si>
     <t>&lt;!--...--&gt;</t>
   </si>
@@ -775,6 +775,63 @@
   </si>
   <si>
     <t>Elapsed Time (Months)</t>
+  </si>
+  <si>
+    <t>Greater than a certain length</t>
+  </si>
+  <si>
+    <t>Get blocks of significant text from the page</t>
+  </si>
+  <si>
+    <t>Significant</t>
+  </si>
+  <si>
+    <t>Not cookie or disclaimer</t>
+  </si>
+  <si>
+    <t>In a link but not a common use link</t>
+  </si>
+  <si>
+    <t>In a heading but not a common use heading</t>
+  </si>
+  <si>
+    <t>Glue together and tf-idf</t>
+  </si>
+  <si>
+    <t>Add weighting to highlighted words</t>
+  </si>
+  <si>
+    <t>Words in headings and significant links</t>
+  </si>
+  <si>
+    <t>Get links from page</t>
+  </si>
+  <si>
+    <t>Identifiy, about us, products/services/news</t>
+  </si>
+  <si>
+    <t>Identify link depth</t>
+  </si>
+  <si>
+    <t>Identify, meaningful domain specific links</t>
+  </si>
+  <si>
+    <t>Follow each link and repeat steps</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Tokenise words, noun phrases, names</t>
+  </si>
+  <si>
+    <t>Entity extract page</t>
+  </si>
+  <si>
+    <t>List of keywords and weightings</t>
+  </si>
+  <si>
+    <t>Remove stop words</t>
   </si>
 </sst>
 </file>
@@ -1244,7 +1301,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D131"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3:D131"/>
     </sheetView>
   </sheetViews>
@@ -3249,12 +3306,115 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="40.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D5" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>260</v>
+      </c>
+      <c r="D9" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>270</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>